<commit_message>
Lot of fixes to prepare delivery
</commit_message>
<xml_diff>
--- a/Subtask5/02-org-ap-ep/04-SHACL/MEP-Bodies-Shapes.xlsx
+++ b/Subtask5/02-org-ap-ep/04-SHACL/MEP-Bodies-Shapes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="293">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -152,34 +152,7 @@
     <t xml:space="preserve">sh:IRI</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/resource/person</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/[0-9]{1,6}$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}$"</t>
   </si>
   <si>
     <t xml:space="preserve">true</t>
@@ -200,34 +173,7 @@
     <t xml:space="preserve">Membership of an MEP (except mandates)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/resource/person/[0-9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]{1,6}/membership/.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}/membership/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:MembershipMandate</t>
@@ -273,34 +219,7 @@
     <t xml:space="preserve">A relation between an Assistant and its MEP. An assistant may assist more than 1 MEP.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/resource/person</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/[0-9]{1,6}/membership/[0-9]{1,6}$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}/membership/[0-9]{1,6}$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:ContactPoint</t>
@@ -315,34 +234,7 @@
     <t xml:space="preserve">Contact Point info for a MEP</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/resource/contact-point/electronic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/[0-9]{1,6}/.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/contact-point/electronic/[0-9]{1,6}/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:PostalAddress</t>
@@ -357,34 +249,7 @@
     <t xml:space="preserve">Postal Address info for a MEP</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/resource/contact-point/place</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/[0-9]{1,6}/.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/contact-point/place/[0-9]{1,6}/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:Organization</t>
@@ -399,34 +264,7 @@
     <t xml:space="preserve">Organization</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/resource/org</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/.*-.*$"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/org/.*-.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">References to external classes</t>
@@ -555,34 +393,7 @@
     <t xml:space="preserve">Organization type</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/org-type/.*$</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/org-type/.*$"</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:CorporateBody</t>
@@ -735,45 +546,13 @@
     <t xml:space="preserve">upper first name</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">org-ep</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:officialFirstName</t>
-    </r>
+    <t xml:space="preserve">org-ep:officialFirstName</t>
   </si>
   <si>
     <t xml:space="preserve">official first name</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">org-ep</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:officialUpperFirstName</t>
-    </r>
+    <t xml:space="preserve">org-ep:officialUpperFirstName</t>
   </si>
   <si>
     <t xml:space="preserve">official upper first name</t>
@@ -791,23 +570,7 @@
     <t xml:space="preserve">upper family name</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">org-ep</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:officialFamilyName</t>
-    </r>
+    <t xml:space="preserve">org-ep:officialFamilyName</t>
   </si>
   <si>
     <t xml:space="preserve">official family name</t>
@@ -837,6 +600,12 @@
     <t xml:space="preserve">birth place</t>
   </si>
   <si>
+    <t xml:space="preserve">org-ep:birthPlaceLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth place label</t>
+  </si>
+  <si>
     <t xml:space="preserve">org-ep:curriculumVitae</t>
   </si>
   <si>
@@ -888,32 +657,7 @@
     <t xml:space="preserve">contact point</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">([sh:node </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">epsh:ContactPoint</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">] [sh:node epsh:PostalAddress])</t>
-    </r>
+    <t xml:space="preserve">([sh:node epsh:ContactPoint] [sh:node epsh:PostalAddress])</t>
   </si>
   <si>
     <t xml:space="preserve">org:hasMembership</t>
@@ -922,32 +666,7 @@
     <t xml:space="preserve">membership</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">([sh:node </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">epsh:MembershipMEP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">] [sh:node epsh:MembershipMandate])</t>
-    </r>
+    <t xml:space="preserve">([sh:node epsh:MembershipMEP] [sh:node epsh:MembershipMandate])</t>
   </si>
   <si>
     <t xml:space="preserve">Constraints on ContactPoint</t>
@@ -1195,7 +914,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1269,11 +988,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1344,7 +1058,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1401,6 +1115,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1415,14 +1133,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1445,19 +1155,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1545,11 +1247,11 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.59"/>
@@ -1765,7 +1467,7 @@
       <c r="J11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="14" t="s">
         <v>43</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1797,7 +1499,7 @@
       <c r="J12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" s="14" t="s">
         <v>50</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1862,13 +1564,13 @@
       <c r="H14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="15" t="s">
         <v>59</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" s="14" t="s">
         <v>43</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1894,13 +1596,13 @@
       <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="15" t="s">
         <v>63</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" s="14" t="s">
         <v>64</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -1917,9 +1619,9 @@
       <c r="B16" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="1" t="s">
         <v>66</v>
       </c>
@@ -1935,7 +1637,7 @@
       <c r="J16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" s="14" t="s">
         <v>69</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -1952,9 +1654,9 @@
       <c r="B17" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="1" t="s">
         <v>71</v>
       </c>
@@ -1970,7 +1672,7 @@
       <c r="J17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" s="14" t="s">
         <v>74</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -2002,7 +1704,7 @@
       <c r="J18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="4" t="s">
         <v>79</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -2015,17 +1717,17 @@
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I19" s="1"/>
     </row>
-    <row r="20" s="16" customFormat="true" ht="32.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+    <row r="20" s="17" customFormat="true" ht="32.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -2047,7 +1749,7 @@
       <c r="J21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="14" t="s">
         <v>84</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -2077,7 +1779,7 @@
       <c r="J22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="14" t="s">
         <v>88</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -2107,7 +1809,7 @@
       <c r="J23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="14" t="s">
         <v>92</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -2137,7 +1839,7 @@
       <c r="J24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="14" t="s">
         <v>96</v>
       </c>
       <c r="L24" s="1" t="s">
@@ -2166,7 +1868,7 @@
       <c r="J25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L25" s="1" t="s">
@@ -2195,7 +1897,7 @@
       <c r="J26" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="K26" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L26" s="1" t="s">
@@ -2224,7 +1926,7 @@
       <c r="J27" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L27" s="1" t="s">
@@ -2253,7 +1955,7 @@
       <c r="J28" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="K28" s="14" t="s">
         <v>112</v>
       </c>
       <c r="L28" s="1" t="s">
@@ -2282,7 +1984,7 @@
       <c r="J29" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="K29" s="14" t="s">
         <v>115</v>
       </c>
       <c r="L29" s="1" t="s">
@@ -2312,7 +2014,7 @@
       <c r="J30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="18" t="s">
+      <c r="K30" s="14" t="s">
         <v>118</v>
       </c>
       <c r="L30" s="1" t="s">
@@ -2342,7 +2044,7 @@
       <c r="J31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="K31" s="14" t="s">
         <v>122</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -2372,7 +2074,7 @@
       <c r="J32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="2" t="s">
         <v>126</v>
       </c>
       <c r="L32" s="1" t="s">
@@ -2390,13 +2092,13 @@
     <hyperlink ref="F10" r:id="rId3" display="rdfs:label@fr"/>
     <hyperlink ref="G10" r:id="rId4" display="rdfs:label@en"/>
     <hyperlink ref="I10" r:id="rId5" display="rdfs:comment@en"/>
-    <hyperlink ref="K11" r:id="rId6" display="http://data.europarl.europa.eu/resource/person"/>
-    <hyperlink ref="K12" r:id="rId7" display="http://data.europarl.europa.eu/resource/person/[0-9"/>
-    <hyperlink ref="K14" r:id="rId8" display="http://data.europarl.europa.eu/resource/person"/>
-    <hyperlink ref="K15" r:id="rId9" display="http://data.europarl.europa.eu/resource/person"/>
-    <hyperlink ref="K16" r:id="rId10" display="http://data.europarl.europa.eu/resource/contact-point/electronic"/>
-    <hyperlink ref="K17" r:id="rId11" display="http://data.europarl.europa.eu/resource/contact-point/place"/>
-    <hyperlink ref="K18" r:id="rId12" display="http://data.europarl.europa.eu/resource/org"/>
+    <hyperlink ref="K11" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}$&quot;"/>
+    <hyperlink ref="K12" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}/membership/.*$&quot;"/>
+    <hyperlink ref="K14" r:id="rId8" display="&quot;^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}$&quot;"/>
+    <hyperlink ref="K15" r:id="rId9" display="&quot;^http://data.europarl.europa.eu/resource/person/[0-9]{1,6}/membership/[0-9]{1,6}$&quot;"/>
+    <hyperlink ref="K16" r:id="rId10" display="&quot;^http://data.europarl.europa.eu/resource/contact-point/electronic/[0-9]{1,6}/.*$&quot;"/>
+    <hyperlink ref="K17" r:id="rId11" display="&quot;^http://data.europarl.europa.eu/resource/contact-point/place/[0-9]{1,6}/.*$&quot;"/>
+    <hyperlink ref="K18" r:id="rId12" display="&quot;^http://data.europarl.europa.eu/resource/org/.*-.*$&quot;"/>
     <hyperlink ref="K21" r:id="rId13" display="&quot;^http://publications.europa.eu/resource/authority/country/.*$&quot;"/>
     <hyperlink ref="K22" r:id="rId14" display="&quot;^http://publications.europa.eu/resource/authority/place/.*$&quot;"/>
     <hyperlink ref="K23" r:id="rId15" display="&quot;^http://data.europarl.europa.eu/authority/civility/.*$&quot;"/>
@@ -2406,8 +2108,8 @@
     <hyperlink ref="K27" r:id="rId19" display="&quot;^http://data.europarl.europa.eu/authority/membership-type/.*$&quot;"/>
     <hyperlink ref="K28" r:id="rId20" display="&quot;^http://data.europarl.europa.eu/authority/function/.*$&quot;"/>
     <hyperlink ref="K29" r:id="rId21" display="&quot;^http://data.europarl.europa.eu/authority/constituency/.*-.*$&quot;"/>
-    <hyperlink ref="K31" r:id="rId22" display="http://data.europarl.europa.eu/authority/org-type/.*$"/>
-    <hyperlink ref="K32" r:id="rId23" display="http://data.europarl.europa.eu/authority/(committee-body"/>
+    <hyperlink ref="K31" r:id="rId22" display="&quot;^http://data.europarl.europa.eu/authority/org-type/.*$&quot;"/>
+    <hyperlink ref="K32" r:id="rId23" display="&quot;^http://data.europarl.europa.eu/authority/(committee-body|delegation-body|institution-body|political-group-body|governance-body)/.*$&quot;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2426,13 +2128,13 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J84" activeCellId="0" sqref="J84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H89" activeCellId="0" sqref="H89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
@@ -2588,34 +2290,34 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>155</v>
       </c>
       <c r="K8" s="12" t="s">
@@ -2630,33 +2332,33 @@
       <c r="N8" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="S8" s="21" t="s">
+      <c r="S8" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="T8" s="21" t="s">
+      <c r="T8" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="U8" s="21" t="s">
+      <c r="U8" s="20" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+    <row r="9" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="T9" s="24"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
@@ -2718,7 +2420,7 @@
       <c r="J11" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="15"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,7 +2428,7 @@
         <f aca="false">CONCATENATE("epsh:P",ROW(A12))</f>
         <v>epsh:P12</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="3" t="s">
         <v>173</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2756,7 +2458,7 @@
         <f aca="false">CONCATENATE("epsh:P",ROW(A13))</f>
         <v>epsh:P13</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="3" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2840,14 +2542,14 @@
       <c r="J15" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="M15" s="14"/>
+      <c r="M15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A16))</f>
         <v>epsh:P16</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2931,7 +2633,7 @@
       <c r="L18" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="M18" s="18"/>
+      <c r="M18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="str">
@@ -2962,7 +2664,7 @@
       <c r="L19" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
@@ -2993,7 +2695,7 @@
       <c r="L20" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="M20" s="18"/>
+      <c r="M20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="str">
@@ -3009,33 +2711,30 @@
       <c r="D21" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="0" t="s">
         <v>192</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="H21" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I21" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="M21" s="18"/>
-      <c r="S21" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="T21" s="26" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A22))</f>
         <v>epsh:P22</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>37</v>
@@ -3044,30 +2743,32 @@
         <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="H22" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="I22" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="M22" s="18"/>
-      <c r="T22" s="26"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>195</v>
+      </c>
+      <c r="M22" s="14"/>
+      <c r="S22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="T22" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A23))</f>
         <v>epsh:P23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>37</v>
@@ -3076,22 +2777,22 @@
         <v>14</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>169</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="M23" s="18"/>
-      <c r="T23" s="26"/>
+        <v>199</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="T23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="str">
@@ -3120,10 +2821,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="M24" s="18"/>
-      <c r="T24" s="26"/>
+        <v>170</v>
+      </c>
+      <c r="M24" s="14"/>
+      <c r="T24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="str">
@@ -3152,10 +2853,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="M25" s="18"/>
-      <c r="T25" s="26"/>
+        <v>199</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="T25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="str">
@@ -3175,7 +2876,7 @@
         <v>205</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>1</v>
@@ -3183,13 +2884,13 @@
       <c r="I26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L26" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="M26" s="18"/>
-      <c r="T26" s="26"/>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="T26" s="24"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A27))</f>
         <v>epsh:P27</v>
@@ -3209,90 +2910,91 @@
       <c r="G27" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="T27" s="26"/>
-    </row>
-    <row r="28" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27" t="str">
+      <c r="H27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="M27" s="14"/>
+      <c r="T27" s="24"/>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A28))</f>
         <v>epsh:P28</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C28" s="14" t="s">
+      <c r="B28" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="0"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="14" t="s">
+      <c r="T28" s="24"/>
+    </row>
+    <row r="29" s="25" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="25" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A29))</f>
+        <v>epsh:P29</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="14"/>
-    </row>
-    <row r="30" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23" t="s">
+      <c r="C29" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="T30" s="24"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A31))</f>
-        <v>epsh:P31</v>
-      </c>
-      <c r="B31" s="0" t="s">
+      <c r="F29" s="15"/>
+      <c r="G29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="15"/>
+    </row>
+    <row r="31" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="G31" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L31" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="M31" s="18"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T31" s="23"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A32))</f>
         <v>epsh:P32</v>
@@ -3304,60 +3006,61 @@
         <v>65</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>216</v>
       </c>
       <c r="G32" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A33))</f>
+        <v>epsh:P33</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="H32" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J32" s="0" t="s">
+      <c r="H33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="0" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="T34" s="24"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A35))</f>
-        <v>epsh:P35</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E35" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="G35" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>170</v>
-      </c>
+      <c r="T35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="str">
@@ -3371,7 +3074,7 @@
         <v>70</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>221</v>
@@ -3401,7 +3104,7 @@
         <v>70</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>223</v>
@@ -3431,13 +3134,13 @@
         <v>70</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>225</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="H38" s="1" t="n">
         <v>0</v>
@@ -3445,10 +3148,9 @@
       <c r="I38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L38" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="M38" s="18"/>
+      <c r="J38" s="0" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="str">
@@ -3462,7 +3164,7 @@
         <v>70</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>227</v>
@@ -3477,9 +3179,9 @@
         <v>1</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="M39" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="M39" s="14"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="str">
@@ -3493,7 +3195,7 @@
         <v>70</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>229</v>
@@ -3508,9 +3210,9 @@
         <v>1</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="M40" s="18"/>
+        <v>85</v>
+      </c>
+      <c r="M40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="str">
@@ -3524,13 +3226,13 @@
         <v>70</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>231</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="H41" s="1" t="n">
         <v>0</v>
@@ -3538,48 +3240,48 @@
       <c r="I41" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="L41" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A42))</f>
+        <v>epsh:P42</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" s="0" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="T45" s="24"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A46))</f>
-        <v>epsh:P46</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="0" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="G46" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H46" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L46" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="M46" s="18"/>
+      <c r="T46" s="23"/>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="str">
@@ -3593,13 +3295,13 @@
         <v>46</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>236</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>1</v>
@@ -3607,10 +3309,10 @@
       <c r="I47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J47" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="M47" s="18"/>
+      <c r="L47" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="M47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="str">
@@ -3624,7 +3326,7 @@
         <v>46</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>238</v>
@@ -3639,11 +3341,11 @@
         <v>1</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="M48" s="18"/>
-    </row>
-    <row r="49" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A49))</f>
         <v>epsh:P49</v>
@@ -3655,16 +3357,13 @@
         <v>46</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="F49" s="14" t="s">
-        <v>241</v>
-      </c>
       <c r="G49" s="0" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="H49" s="1" t="n">
         <v>1</v>
@@ -3672,26 +3371,29 @@
       <c r="I49" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M49" s="18"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J49" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A50))</f>
         <v>epsh:P50</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E50" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>243</v>
       </c>
       <c r="G50" s="0" t="s">
@@ -3703,12 +3405,12 @@
       <c r="I50" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L50" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="M50" s="18"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A51))</f>
         <v>epsh:P51</v>
@@ -3720,7 +3422,7 @@
         <v>46</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>245</v>
@@ -3735,49 +3437,49 @@
         <v>1</v>
       </c>
       <c r="L51" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A52))</f>
+        <v>epsh:P52</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L52" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="M51" s="18"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M52" s="18"/>
-    </row>
-    <row r="53" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="T53" s="24"/>
-    </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A54))</f>
-        <v>epsh:P54</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H54" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M54" s="18"/>
-      <c r="U54" s="18" t="s">
-        <v>247</v>
-      </c>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="T54" s="23"/>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="str">
@@ -3791,13 +3493,13 @@
         <v>51</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>236</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="H55" s="1" t="n">
         <v>1</v>
@@ -3805,10 +3507,10 @@
       <c r="I55" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J55" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="M55" s="18"/>
+      <c r="M55" s="14"/>
+      <c r="U55" s="14" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="str">
@@ -3822,7 +3524,7 @@
         <v>51</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>238</v>
@@ -3837,11 +3539,11 @@
         <v>1</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="M56" s="18"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+      <c r="M56" s="14"/>
+    </row>
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A57))</f>
         <v>epsh:P57</v>
@@ -3853,13 +3555,13 @@
         <v>51</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="H57" s="1" t="n">
         <v>1</v>
@@ -3867,10 +3569,10 @@
       <c r="I57" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L57" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="M57" s="18"/>
+      <c r="J57" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="M57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="str">
@@ -3878,16 +3580,16 @@
         <v>epsh:P58</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>42</v>
@@ -3899,42 +3601,42 @@
         <v>1</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="M58" s="18"/>
-    </row>
-    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+      <c r="M58" s="14"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A59))</f>
         <v>epsh:P59</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>42</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="M59" s="18"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="M59" s="14"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A60))</f>
         <v>epsh:P60</v>
@@ -3946,24 +3648,24 @@
         <v>51</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>252</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J60" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="M60" s="18"/>
+      <c r="L60" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="str">
@@ -3992,9 +3694,9 @@
         <v>1</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="M61" s="18"/>
+        <v>170</v>
+      </c>
+      <c r="M61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="str">
@@ -4002,7 +3704,7 @@
         <v>epsh:P62</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>51</v>
@@ -4011,7 +3713,7 @@
         <v>9</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G62" s="0" t="s">
         <v>169</v>
@@ -4023,46 +3725,47 @@
         <v>1</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="M62" s="18"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="M62" s="14"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A63))</f>
+        <v>epsh:P63</v>
+      </c>
+      <c r="B63" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="T64" s="24"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A65))</f>
-        <v>epsh:P65</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D65" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="G65" s="0" t="s">
+      <c r="C63" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="G63" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="H65" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>170</v>
-      </c>
+      <c r="H63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="T65" s="23"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="str">
@@ -4070,16 +3773,16 @@
         <v>epsh:P66</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>169</v>
@@ -4100,16 +3803,16 @@
         <v>epsh:P67</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>172</v>
+        <v>2</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>178</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>169</v>
@@ -4123,25 +3826,23 @@
       <c r="J67" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="M67" s="14"/>
-      <c r="R67" s="1"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A68))</f>
         <v>epsh:P68</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>180</v>
+        <v>3</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>169</v>
@@ -4155,7 +3856,8 @@
       <c r="J68" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="M68" s="14"/>
+      <c r="M68" s="15"/>
+      <c r="R68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="str">
@@ -4163,19 +3865,19 @@
         <v>epsh:P69</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>259</v>
+        <v>179</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="H69" s="1" t="n">
         <v>1</v>
@@ -4183,9 +3885,10 @@
       <c r="I69" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R69" s="18" t="s">
-        <v>261</v>
-      </c>
+      <c r="J69" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="M69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="str">
@@ -4193,19 +3896,19 @@
         <v>epsh:P70</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>198</v>
+        <v>261</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>199</v>
+        <v>5</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>262</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="H70" s="1" t="n">
         <v>1</v>
@@ -4213,8 +3916,8 @@
       <c r="I70" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J70" s="0" t="s">
-        <v>170</v>
+      <c r="R70" s="14" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4223,86 +3926,82 @@
         <v>epsh:P71</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D71" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A72))</f>
+        <v>epsh:P72</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E71" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H71" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L71" s="0" t="s">
+      <c r="E72" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H72" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L72" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M72" s="18"/>
-    </row>
-    <row r="74" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="T74" s="24"/>
-    </row>
-    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A75))</f>
-        <v>epsh:P75</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D75" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="G75" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H75" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M75" s="18"/>
-      <c r="U75" s="18" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M73" s="14"/>
+    </row>
+    <row r="75" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="T75" s="23"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A76))</f>
         <v>epsh:P76</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>42</v>
@@ -4313,81 +4012,87 @@
       <c r="I76" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K76" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L76" s="28"/>
-      <c r="M76" s="18"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M76" s="14"/>
+      <c r="U76" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A77))</f>
         <v>epsh:P77</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D77" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L77" s="3"/>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A78))</f>
+        <v>epsh:P78</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E77" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H77" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I77" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L77" s="0" t="s">
+      <c r="E78" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L78" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="M77" s="18"/>
-      <c r="U77" s="18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="79" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="T79" s="24"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="str">
-        <f aca="false">CONCATENATE("epsh:P",ROW(A80))</f>
-        <v>epsh:P80</v>
-      </c>
-      <c r="B80" s="0" t="s">
+      <c r="M78" s="14"/>
+      <c r="U78" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D80" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E80" s="1" t="s">
+    </row>
+    <row r="80" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="G80" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H80" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I80" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q80" s="1"/>
-    </row>
-    <row r="81" customFormat="false" ht="85.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T80" s="23"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A81))</f>
         <v>epsh:P81</v>
@@ -4399,61 +4104,58 @@
         <v>75</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E81" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="G81" s="0" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="H81" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I81" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M81" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="N81" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="R81" s="29"/>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="85.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A82))</f>
         <v>epsh:P82</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>235</v>
+      <c r="B82" s="0" t="s">
+        <v>272</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D82" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H82" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I82" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E82" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H82" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I82" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="R82" s="18"/>
+      <c r="M82" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="N82" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="R82" s="26"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="str">
@@ -4467,59 +4169,53 @@
         <v>75</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G83" s="0" t="s">
+      <c r="G83" s="3" t="s">
         <v>169</v>
       </c>
       <c r="H83" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J83" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J83" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="R83" s="14"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A84))</f>
         <v>epsh:P84</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>275</v>
+      <c r="B84" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="G84" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G84" s="0" t="s">
         <v>169</v>
       </c>
       <c r="H84" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" s="0" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="R84" s="18"/>
-      <c r="S84" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="T84" s="1" t="s">
-        <v>277</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,30 +4223,40 @@
         <f aca="false">CONCATENATE("epsh:P",ROW(A85))</f>
         <v>epsh:P85</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>278</v>
+      <c r="B85" s="0" t="s">
+        <v>277</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="H85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>24</v>
+      </c>
       <c r="J85" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
+      </c>
+      <c r="R85" s="14"/>
+      <c r="S85" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="T85" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="str">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A86))</f>
         <v>epsh:P86</v>
       </c>
@@ -4561,24 +4267,20 @@
         <v>75</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="G86" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H86" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I86" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L86" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="R86" s="18"/>
+      <c r="G86" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T86" s="1" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="str">
@@ -4586,19 +4288,19 @@
         <v>epsh:P87</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>169</v>
+        <v>283</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="H87" s="1" t="n">
         <v>1</v>
@@ -4606,10 +4308,10 @@
       <c r="I87" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J87" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="R87" s="18"/>
+      <c r="L87" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="R87" s="14"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="str">
@@ -4617,19 +4319,19 @@
         <v>epsh:P88</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>283</v>
+        <v>253</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="G88" s="0" t="s">
-        <v>42</v>
+      <c r="G88" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="H88" s="1" t="n">
         <v>1</v>
@@ -4637,77 +4339,107 @@
       <c r="I88" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L88" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J88" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="R88" s="14"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A89))</f>
         <v>epsh:P89</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="3" t="s">
         <v>285</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="F89" s="14" t="s">
-        <v>287</v>
-      </c>
       <c r="G89" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K89" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L89" s="3"/>
-      <c r="M89" s="1"/>
-      <c r="R89" s="18"/>
-    </row>
-    <row r="90" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L89" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A90))</f>
         <v>epsh:P90</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E90" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F90" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="F90" s="14" t="s">
-        <v>287</v>
-      </c>
       <c r="G90" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="I90" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L90" s="3"/>
-    </row>
-    <row r="104" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L104" s="0" t="s">
+      <c r="M90" s="1"/>
+      <c r="R90" s="14"/>
+    </row>
+    <row r="91" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="3" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A91))</f>
+        <v>epsh:P91</v>
+      </c>
+      <c r="B91" s="0" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C91" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D91" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L91" s="3"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L105" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4717,10 +4449,10 @@
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes/meps"/>
     <hyperlink ref="C3" r:id="rId2" display="http://data.europarl.europa.eu/ontology/org-ep#"/>
     <hyperlink ref="E8" r:id="rId3" display="sh:name@en"/>
-    <hyperlink ref="U54" r:id="rId4" display="http://data.europarl.europa.eu/authority/membership-type/MANDATE"/>
-    <hyperlink ref="R69" r:id="rId5" display="( &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA-GRP&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-LOC&gt; )"/>
-    <hyperlink ref="U75" r:id="rId6" display="http://data.europarl.europa.eu/authority/membership-type/PERSON"/>
-    <hyperlink ref="U77" r:id="rId7" display="http://data.europarl.europa.eu/authority/function/ASSISTANT"/>
+    <hyperlink ref="U55" r:id="rId4" display="http://data.europarl.europa.eu/authority/membership-type/MANDATE"/>
+    <hyperlink ref="R70" r:id="rId5" display="( &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA-GRP&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-LOC&gt; )"/>
+    <hyperlink ref="U76" r:id="rId6" display="http://data.europarl.europa.eu/authority/membership-type/PERSON"/>
+    <hyperlink ref="U78" r:id="rId7" display="http://data.europarl.europa.eu/authority/function/ASSISTANT"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
MEP constituencyLabel + SHACL
</commit_message>
<xml_diff>
--- a/Subtask5/02-org-ap-ep/04-SHACL/MEP-Bodies-Shapes.xlsx
+++ b/Subtask5/02-org-ap-ep/04-SHACL/MEP-Bodies-Shapes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="292">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -164,6 +164,14 @@
     <t xml:space="preserve">epsh:MembershipMEP</t>
   </si>
   <si>
+    <t xml:space="preserve">PREFIX org: &lt;http://www.w3.org/ns/org#&gt;
+PREFIX org-ep: &lt;http://data.europarl.europa.eu/ontology/org-ep#&gt;
+SELECT ?this WHERE {
+ ?this a org-ep:Membership .
+ MINUS { ?this org-ep:hasMembershipType &lt;http://data.europarl.europa.eu/authority/membership-type/PERSON&gt; }
+}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Appartenance MEP</t>
   </si>
   <si>
@@ -177,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">epsh:MembershipMandate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org-ep:MembershipMandate</t>
   </si>
   <si>
     <t xml:space="preserve">Mandat MEP</t>
@@ -366,15 +377,6 @@
     <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/function/.*$"</t>
   </si>
   <si>
-    <t xml:space="preserve">epsh:Constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/constituency/.*-.*$"</t>
-  </si>
-  <si>
     <t xml:space="preserve">epsh:Site</t>
   </si>
   <si>
@@ -780,10 +782,10 @@
     <t xml:space="preserve">country</t>
   </si>
   <si>
-    <t xml:space="preserve">org-ep:constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constituency</t>
+    <t xml:space="preserve">org-ep:constituencyLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constituency label</t>
   </si>
   <si>
     <t xml:space="preserve">dc:identifier</t>
@@ -1247,11 +1249,11 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.59"/>
@@ -1477,30 +1479,37 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="D12" s="1" t="str">
+        <f aca="false">CONCATENATE(A12,"-target")</f>
+        <v>epsh:MembershipMEP-target</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>44</v>
@@ -1511,28 +1520,31 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>44</v>
@@ -1543,7 +1555,7 @@
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>38</v>
@@ -1553,19 +1565,19 @@
         <v>epsh:Assistant-target</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>42</v>
@@ -1582,28 +1594,28 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>44</v>
@@ -1614,7 +1626,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>38</v>
@@ -1623,22 +1635,22 @@
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>6</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>44</v>
@@ -1649,7 +1661,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>38</v>
@@ -1658,22 +1670,22 @@
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>44</v>
@@ -1684,19 +1696,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>8</v>
@@ -1705,7 +1717,7 @@
         <v>42</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>44</v>
@@ -1719,7 +1731,7 @@
     </row>
     <row r="20" s="17" customFormat="true" ht="32.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -1731,16 +1743,16 @@
     </row>
     <row r="21" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>10</v>
@@ -1750,7 +1762,7 @@
         <v>42</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>44</v>
@@ -1761,16 +1773,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>11</v>
@@ -1780,7 +1792,7 @@
         <v>42</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>44</v>
@@ -1791,16 +1803,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>12</v>
@@ -1810,7 +1822,7 @@
         <v>42</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>44</v>
@@ -1821,16 +1833,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>13</v>
@@ -1840,7 +1852,7 @@
         <v>42</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>44</v>
@@ -1851,16 +1863,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>14</v>
@@ -1869,7 +1881,7 @@
         <v>42</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>44</v>
@@ -1880,16 +1892,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>15</v>
@@ -1898,7 +1910,7 @@
         <v>42</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>44</v>
@@ -1909,16 +1921,16 @@
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>16</v>
@@ -1927,7 +1939,7 @@
         <v>42</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>44</v>
@@ -1938,16 +1950,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>17</v>
@@ -1956,7 +1968,7 @@
         <v>42</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>44</v>
@@ -1965,27 +1977,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="J29" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>44</v>
@@ -1996,26 +2009,26 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>117</v>
+      <c r="F30" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>44</v>
@@ -2026,26 +2039,26 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>120</v>
+      <c r="F31" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K31" s="14" t="s">
-        <v>122</v>
+      <c r="K31" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>44</v>
@@ -2054,36 +2067,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
@@ -2107,9 +2091,8 @@
     <hyperlink ref="K26" r:id="rId18" display="&quot;^http://data.europarl.europa.eu/authority/parliamentary-term/[0-9][0-9]?$&quot;"/>
     <hyperlink ref="K27" r:id="rId19" display="&quot;^http://data.europarl.europa.eu/authority/membership-type/.*$&quot;"/>
     <hyperlink ref="K28" r:id="rId20" display="&quot;^http://data.europarl.europa.eu/authority/function/.*$&quot;"/>
-    <hyperlink ref="K29" r:id="rId21" display="&quot;^http://data.europarl.europa.eu/authority/constituency/.*-.*$&quot;"/>
-    <hyperlink ref="K31" r:id="rId22" display="&quot;^http://data.europarl.europa.eu/authority/org-type/.*$&quot;"/>
-    <hyperlink ref="K32" r:id="rId23" display="&quot;^http://data.europarl.europa.eu/authority/(committee-body|delegation-body|institution-body|political-group-body|governance-body)/.*$&quot;"/>
+    <hyperlink ref="K30" r:id="rId21" display="&quot;^http://data.europarl.europa.eu/authority/org-type/.*$&quot;"/>
+    <hyperlink ref="K31" r:id="rId22" display="&quot;^http://data.europarl.europa.eu/authority/(committee-body|delegation-body|institution-body|political-group-body|governance-body)/.*$&quot;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2128,13 +2111,13 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H89" activeCellId="0" sqref="H89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="L60" activeCellId="0" sqref="L60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
@@ -2197,7 +2180,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -2226,67 +2209,67 @@
     </row>
     <row r="7" s="11" customFormat="true" ht="73.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="M7" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="N7" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="R7" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="S7" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="T7" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="T7" s="11" t="s">
+      <c r="U7" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,69 +2277,69 @@
         <v>25</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>150</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>151</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>152</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="J8" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="L8" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>157</v>
       </c>
       <c r="M8" s="12" t="s">
         <v>34</v>
       </c>
       <c r="N8" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="P8" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="Q8" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="R8" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="S8" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="T8" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="U8" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="U8" s="20" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="9" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T9" s="23"/>
     </row>
@@ -2366,7 +2349,7 @@
         <v>epsh:P10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
@@ -2375,19 +2358,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="H10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="R10" s="1"/>
     </row>
@@ -2397,7 +2380,7 @@
         <v>epsh:P11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>37</v>
@@ -2406,19 +2389,19 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G11" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M11" s="15"/>
       <c r="R11" s="1"/>
@@ -2429,7 +2412,7 @@
         <v>epsh:P12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>37</v>
@@ -2438,10 +2421,10 @@
         <v>3</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
@@ -2450,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,7 +2442,7 @@
         <v>epsh:P13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
@@ -2468,10 +2451,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
@@ -2480,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2489,7 +2472,7 @@
         <v>epsh:P14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>37</v>
@@ -2498,19 +2481,19 @@
         <v>5</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G14" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2519,7 +2502,7 @@
         <v>epsh:P15</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>37</v>
@@ -2528,19 +2511,19 @@
         <v>6</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G15" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M15" s="15"/>
     </row>
@@ -2550,7 +2533,7 @@
         <v>epsh:P16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>37</v>
@@ -2559,10 +2542,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
@@ -2571,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,7 +2563,7 @@
         <v>epsh:P17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>37</v>
@@ -2589,10 +2572,10 @@
         <v>8</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
@@ -2601,7 +2584,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2593,7 @@
         <v>epsh:P18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>37</v>
@@ -2619,7 +2602,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>42</v>
@@ -2631,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M18" s="14"/>
     </row>
@@ -2641,7 +2624,7 @@
         <v>epsh:P19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>37</v>
@@ -2650,7 +2633,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>42</v>
@@ -2662,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M19" s="14"/>
     </row>
@@ -2672,7 +2655,7 @@
         <v>epsh:P20</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>37</v>
@@ -2681,7 +2664,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>42</v>
@@ -2693,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M20" s="14"/>
     </row>
@@ -2703,7 +2686,7 @@
         <v>epsh:P21</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>37</v>
@@ -2712,10 +2695,10 @@
         <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
@@ -2724,7 +2707,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M21" s="14"/>
     </row>
@@ -2734,7 +2717,7 @@
         <v>epsh:P22</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>37</v>
@@ -2743,23 +2726,23 @@
         <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M22" s="14"/>
       <c r="S22" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T22" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,7 +2751,7 @@
         <v>epsh:P23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>37</v>
@@ -2777,10 +2760,10 @@
         <v>14</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0</v>
@@ -2789,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M23" s="14"/>
       <c r="T23" s="24"/>
@@ -2800,7 +2783,7 @@
         <v>epsh:P24</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>37</v>
@@ -2809,19 +2792,19 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G24" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M24" s="14"/>
       <c r="T24" s="24"/>
@@ -2832,7 +2815,7 @@
         <v>epsh:P25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>37</v>
@@ -2841,10 +2824,10 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>1</v>
@@ -2853,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M25" s="14"/>
       <c r="T25" s="24"/>
@@ -2864,7 +2847,7 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>37</v>
@@ -2873,19 +2856,19 @@
         <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G26" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M26" s="14"/>
       <c r="T26" s="24"/>
@@ -2896,7 +2879,7 @@
         <v>epsh:P27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>37</v>
@@ -2905,7 +2888,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>42</v>
@@ -2917,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M27" s="14"/>
       <c r="T27" s="24"/>
@@ -2928,7 +2911,7 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>37</v>
@@ -2937,7 +2920,7 @@
         <v>19</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>42</v>
@@ -2945,7 +2928,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="14"/>
       <c r="N28" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T28" s="24"/>
     </row>
@@ -2955,7 +2938,7 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>37</v>
@@ -2964,7 +2947,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="3" t="s">
@@ -2979,7 +2962,7 @@
       <c r="L29" s="0"/>
       <c r="M29" s="14"/>
       <c r="N29" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -2990,7 +2973,7 @@
     </row>
     <row r="31" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T31" s="23"/>
     </row>
@@ -3000,17 +2983,17 @@
         <v>epsh:P32</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>216</v>
-      </c>
       <c r="G32" s="0" t="s">
         <v>42</v>
       </c>
@@ -3021,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M32" s="14"/>
     </row>
@@ -3031,34 +3014,34 @@
         <v>epsh:P33</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G33" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T35" s="23"/>
     </row>
@@ -3068,19 +3051,19 @@
         <v>epsh:P36</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>0</v>
@@ -3089,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,19 +3081,19 @@
         <v>epsh:P37</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H37" s="1" t="n">
         <v>0</v>
@@ -3119,7 +3102,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3128,19 +3111,19 @@
         <v>epsh:P38</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H38" s="1" t="n">
         <v>0</v>
@@ -3149,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,16 +3141,16 @@
         <v>epsh:P39</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>42</v>
@@ -3179,7 +3162,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M39" s="14"/>
     </row>
@@ -3189,16 +3172,16 @@
         <v>epsh:P40</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>42</v>
@@ -3210,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M40" s="14"/>
     </row>
@@ -3220,16 +3203,16 @@
         <v>epsh:P41</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>42</v>
@@ -3241,7 +3224,7 @@
         <v>1</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M41" s="14"/>
     </row>
@@ -3251,19 +3234,19 @@
         <v>epsh:P42</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H42" s="1" t="n">
         <v>0</v>
@@ -3272,14 +3255,14 @@
         <v>1</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T46" s="23"/>
     </row>
@@ -3289,7 +3272,7 @@
         <v>epsh:P47</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>46</v>
@@ -3298,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>42</v>
@@ -3310,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M47" s="14"/>
     </row>
@@ -3320,7 +3303,7 @@
         <v>epsh:P48</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>46</v>
@@ -3329,10 +3312,10 @@
         <v>2</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H48" s="1" t="n">
         <v>1</v>
@@ -3341,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M48" s="14"/>
     </row>
@@ -3351,7 +3334,7 @@
         <v>epsh:P49</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>46</v>
@@ -3360,10 +3343,10 @@
         <v>3</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H49" s="1" t="n">
         <v>1</v>
@@ -3372,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M49" s="14"/>
     </row>
@@ -3382,7 +3365,7 @@
         <v>epsh:P50</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>46</v>
@@ -3391,11 +3374,11 @@
         <v>4</v>
       </c>
       <c r="E50" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="F50" s="15" t="s">
-        <v>243</v>
-      </c>
       <c r="G50" s="0" t="s">
         <v>42</v>
       </c>
@@ -3406,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M50" s="14"/>
     </row>
@@ -3416,7 +3399,7 @@
         <v>epsh:P51</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>46</v>
@@ -3425,7 +3408,7 @@
         <v>5</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>42</v>
@@ -3437,7 +3420,7 @@
         <v>1</v>
       </c>
       <c r="L51" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M51" s="14"/>
     </row>
@@ -3447,7 +3430,7 @@
         <v>epsh:P52</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>46</v>
@@ -3456,7 +3439,7 @@
         <v>8</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>42</v>
@@ -3468,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="L52" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M52" s="14"/>
     </row>
@@ -3477,7 +3460,7 @@
     </row>
     <row r="54" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T54" s="23"/>
     </row>
@@ -3487,16 +3470,16 @@
         <v>epsh:P55</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>235</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>236</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>42</v>
@@ -3509,7 +3492,7 @@
       </c>
       <c r="M55" s="14"/>
       <c r="U55" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3518,19 +3501,19 @@
         <v>epsh:P56</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H56" s="1" t="n">
         <v>1</v>
@@ -3539,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M56" s="14"/>
     </row>
@@ -3549,19 +3532,19 @@
         <v>epsh:P57</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H57" s="1" t="n">
         <v>1</v>
@@ -3570,7 +3553,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M57" s="14"/>
     </row>
@@ -3580,16 +3563,16 @@
         <v>epsh:P58</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>42</v>
@@ -3601,7 +3584,7 @@
         <v>1</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M58" s="14"/>
     </row>
@@ -3611,16 +3594,16 @@
         <v>epsh:P59</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>42</v>
@@ -3632,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M59" s="14"/>
     </row>
@@ -3642,19 +3625,19 @@
         <v>epsh:P60</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>42</v>
+        <v>168</v>
       </c>
       <c r="H60" s="1" t="n">
         <v>0</v>
@@ -3662,8 +3645,8 @@
       <c r="I60" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L60" s="0" t="s">
-        <v>113</v>
+      <c r="J60" s="0" t="s">
+        <v>169</v>
       </c>
       <c r="M60" s="14"/>
     </row>
@@ -3673,28 +3656,28 @@
         <v>epsh:P61</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G61" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H61" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M61" s="14"/>
     </row>
@@ -3704,28 +3687,25 @@
         <v>epsh:P62</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E62" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" s="0" t="s">
         <v>256</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="H62" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>257</v>
       </c>
       <c r="M62" s="14"/>
     </row>
@@ -3735,35 +3715,32 @@
         <v>epsh:P63</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="H63" s="1" t="n">
-        <v>1</v>
+        <v>168</v>
       </c>
       <c r="I63" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M63" s="14"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="65" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="T65" s="23"/>
     </row>
@@ -3773,28 +3750,28 @@
         <v>epsh:P66</v>
       </c>
       <c r="B66" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D66" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E66" s="0" t="s">
+      <c r="G66" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="G66" s="0" t="s">
+      <c r="H66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H66" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3803,28 +3780,28 @@
         <v>epsh:P67</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G67" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H67" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H67" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,28 +3810,28 @@
         <v>epsh:P68</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G68" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H68" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M68" s="15"/>
       <c r="R68" s="1"/>
@@ -3865,28 +3842,28 @@
         <v>epsh:P69</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G69" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H69" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I69" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="M69" s="15"/>
     </row>
@@ -3896,28 +3873,28 @@
         <v>epsh:P70</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E70" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H70" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R70" s="14" t="s">
         <v>262</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H70" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R70" s="14" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,28 +3903,28 @@
         <v>epsh:P71</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G71" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H71" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I71" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,16 +3933,16 @@
         <v>epsh:P72</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>42</v>
@@ -3974,7 +3951,7 @@
         <v>1</v>
       </c>
       <c r="L72" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3982,7 +3959,7 @@
     </row>
     <row r="75" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="T75" s="23"/>
     </row>
@@ -3992,16 +3969,16 @@
         <v>epsh:P76</v>
       </c>
       <c r="B76" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" s="0" t="s">
         <v>235</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D76" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>236</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>42</v>
@@ -4014,7 +3991,7 @@
       </c>
       <c r="M76" s="14"/>
       <c r="U76" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4023,10 +4000,10 @@
         <v>epsh:P77</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>2</v>
@@ -4035,7 +4012,7 @@
         <v>40</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>42</v>
@@ -4058,16 +4035,16 @@
         <v>epsh:P78</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G78" s="0" t="s">
         <v>42</v>
@@ -4079,16 +4056,16 @@
         <v>1</v>
       </c>
       <c r="L78" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M78" s="14"/>
       <c r="U78" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T80" s="23"/>
     </row>
@@ -4098,16 +4075,16 @@
         <v>epsh:P81</v>
       </c>
       <c r="B81" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D81" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="G81" s="0" t="s">
         <v>42</v>
@@ -4126,22 +4103,22 @@
         <v>epsh:P82</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E82" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="G82" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H82" s="1" t="n">
         <v>2</v>
@@ -4150,10 +4127,10 @@
         <v>3</v>
       </c>
       <c r="M82" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="N82" s="15" t="s">
         <v>275</v>
-      </c>
-      <c r="N82" s="15" t="s">
-        <v>276</v>
       </c>
       <c r="R82" s="26"/>
     </row>
@@ -4163,19 +4140,19 @@
         <v>epsh:P83</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D83" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H83" s="1" t="n">
         <v>1</v>
@@ -4184,7 +4161,7 @@
         <v>1</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R83" s="14"/>
     </row>
@@ -4194,19 +4171,19 @@
         <v>epsh:P84</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D84" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H84" s="1" t="n">
         <v>0</v>
@@ -4215,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,19 +4201,19 @@
         <v>epsh:P85</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D85" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H85" s="1" t="n">
         <v>1</v>
@@ -4245,14 +4222,14 @@
         <v>24</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="R85" s="14"/>
       <c r="S85" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T85" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,25 +4238,25 @@
         <v>epsh:P86</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D86" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T86" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4288,16 +4265,16 @@
         <v>epsh:P87</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G87" s="0" t="s">
         <v>42</v>
@@ -4309,7 +4286,7 @@
         <v>1</v>
       </c>
       <c r="L87" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R87" s="14"/>
     </row>
@@ -4319,28 +4296,28 @@
         <v>epsh:P88</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G88" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H88" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="H88" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I88" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="R88" s="14"/>
     </row>
@@ -4350,16 +4327,16 @@
         <v>epsh:P89</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D89" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G89" s="0" t="s">
         <v>42</v>
@@ -4371,7 +4348,7 @@
         <v>1</v>
       </c>
       <c r="L89" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4380,25 +4357,25 @@
         <v>epsh:P90</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E90" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="F90" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="F90" s="15" t="s">
-        <v>289</v>
-      </c>
       <c r="G90" s="0" t="s">
         <v>42</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L90" s="3"/>
       <c r="M90" s="1"/>
@@ -4410,19 +4387,19 @@
         <v>epsh:P91</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>11</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F91" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G91" s="0" t="s">
         <v>42</v>
@@ -4431,13 +4408,13 @@
         <v>1</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L91" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L105" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>